<commit_message>
added auto cleaning, handled special chracters like $, data can be stored in numrics, text, boolean, datetime etc
</commit_message>
<xml_diff>
--- a/files/DummyData.xlsx
+++ b/files/DummyData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="360" windowWidth="14980" windowHeight="7020" activeTab="4"/>
+    <workbookView xWindow="400" yWindow="360" windowWidth="14980" windowHeight="7020"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -1841,8 +1841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3138,8 +3138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G140"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>